<commit_message>
02.01.2020 New Year first Sales Update
</commit_message>
<xml_diff>
--- a/2020/December/All Details/31.12.2020/MC Bank Statement Dec-2020.xlsx
+++ b/2020/December/All Details/31.12.2020/MC Bank Statement Dec-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 2020" sheetId="7" r:id="rId1"/>
@@ -3062,12 +3062,51 @@
     <xf numFmtId="0" fontId="4" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3078,45 +3117,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="39" fillId="35" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3282,7 +3282,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3294,7 +3294,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3317,14 +3317,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3412,7 +3412,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3424,7 +3424,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3447,14 +3447,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3486,7 +3486,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3498,7 +3498,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3521,14 +3521,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -5043,11 +5043,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z320"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="10" ySplit="13" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="10" ySplit="13" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="S37" sqref="S37"/>
+      <selection pane="bottomRight" activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5059,73 +5059,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="300" t="s">
+      <c r="A1" s="294" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="300"/>
-      <c r="C1" s="300"/>
-      <c r="D1" s="300"/>
-      <c r="E1" s="300"/>
-      <c r="F1" s="300"/>
-      <c r="G1" s="300"/>
-      <c r="H1" s="300"/>
-      <c r="I1" s="300"/>
-      <c r="J1" s="300"/>
-      <c r="K1" s="300"/>
-      <c r="L1" s="300"/>
-      <c r="M1" s="300"/>
-      <c r="N1" s="300"/>
-      <c r="O1" s="300"/>
-      <c r="P1" s="300"/>
-      <c r="Q1" s="300"/>
-      <c r="R1" s="300"/>
-      <c r="S1" s="300"/>
+      <c r="B1" s="294"/>
+      <c r="C1" s="294"/>
+      <c r="D1" s="294"/>
+      <c r="E1" s="294"/>
+      <c r="F1" s="294"/>
+      <c r="G1" s="294"/>
+      <c r="H1" s="294"/>
+      <c r="I1" s="294"/>
+      <c r="J1" s="294"/>
+      <c r="K1" s="294"/>
+      <c r="L1" s="294"/>
+      <c r="M1" s="294"/>
+      <c r="N1" s="294"/>
+      <c r="O1" s="294"/>
+      <c r="P1" s="294"/>
+      <c r="Q1" s="294"/>
+      <c r="R1" s="294"/>
+      <c r="S1" s="294"/>
     </row>
     <row r="2" spans="1:26" s="203" customFormat="1" ht="18">
-      <c r="A2" s="301" t="s">
+      <c r="A2" s="295" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="301"/>
-      <c r="C2" s="301"/>
-      <c r="D2" s="301"/>
-      <c r="E2" s="301"/>
-      <c r="F2" s="301"/>
-      <c r="G2" s="301"/>
-      <c r="H2" s="301"/>
-      <c r="I2" s="301"/>
-      <c r="J2" s="301"/>
-      <c r="K2" s="301"/>
-      <c r="L2" s="301"/>
-      <c r="M2" s="301"/>
-      <c r="N2" s="301"/>
-      <c r="O2" s="301"/>
-      <c r="P2" s="301"/>
-      <c r="Q2" s="301"/>
-      <c r="R2" s="301"/>
-      <c r="S2" s="301"/>
+      <c r="B2" s="295"/>
+      <c r="C2" s="295"/>
+      <c r="D2" s="295"/>
+      <c r="E2" s="295"/>
+      <c r="F2" s="295"/>
+      <c r="G2" s="295"/>
+      <c r="H2" s="295"/>
+      <c r="I2" s="295"/>
+      <c r="J2" s="295"/>
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="M2" s="295"/>
+      <c r="N2" s="295"/>
+      <c r="O2" s="295"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
+      <c r="S2" s="295"/>
     </row>
     <row r="3" spans="1:26" s="204" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A3" s="302" t="s">
+      <c r="A3" s="296" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="303"/>
-      <c r="C3" s="303"/>
-      <c r="D3" s="303"/>
-      <c r="E3" s="303"/>
-      <c r="F3" s="303"/>
-      <c r="G3" s="303"/>
-      <c r="H3" s="303"/>
-      <c r="I3" s="303"/>
-      <c r="J3" s="303"/>
-      <c r="K3" s="303"/>
-      <c r="L3" s="303"/>
-      <c r="M3" s="303"/>
-      <c r="N3" s="303"/>
-      <c r="O3" s="303"/>
-      <c r="P3" s="303"/>
-      <c r="Q3" s="303"/>
-      <c r="R3" s="303"/>
-      <c r="S3" s="304"/>
+      <c r="B3" s="297"/>
+      <c r="C3" s="297"/>
+      <c r="D3" s="297"/>
+      <c r="E3" s="297"/>
+      <c r="F3" s="297"/>
+      <c r="G3" s="297"/>
+      <c r="H3" s="297"/>
+      <c r="I3" s="297"/>
+      <c r="J3" s="297"/>
+      <c r="K3" s="297"/>
+      <c r="L3" s="297"/>
+      <c r="M3" s="297"/>
+      <c r="N3" s="297"/>
+      <c r="O3" s="297"/>
+      <c r="P3" s="297"/>
+      <c r="Q3" s="297"/>
+      <c r="R3" s="297"/>
+      <c r="S3" s="298"/>
       <c r="U3" s="116"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
@@ -5134,58 +5134,58 @@
       <c r="Z3" s="29"/>
     </row>
     <row r="4" spans="1:26" s="206" customFormat="1">
-      <c r="A4" s="305" t="s">
+      <c r="A4" s="299" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="307" t="s">
+      <c r="B4" s="301" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="294" t="s">
+      <c r="C4" s="303" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="294" t="s">
+      <c r="D4" s="303" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="294" t="s">
+      <c r="E4" s="303" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="294" t="s">
+      <c r="F4" s="303" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="294" t="s">
+      <c r="G4" s="303" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="294" t="s">
+      <c r="H4" s="303" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="294" t="s">
+      <c r="I4" s="303" t="s">
         <v>132</v>
       </c>
-      <c r="J4" s="294" t="s">
+      <c r="J4" s="303" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="294" t="s">
+      <c r="K4" s="303" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="294" t="s">
+      <c r="L4" s="303" t="s">
         <v>110</v>
       </c>
-      <c r="M4" s="294" t="s">
+      <c r="M4" s="303" t="s">
         <v>111</v>
       </c>
-      <c r="N4" s="294" t="s">
+      <c r="N4" s="303" t="s">
         <v>112</v>
       </c>
-      <c r="O4" s="296" t="s">
+      <c r="O4" s="309" t="s">
         <v>212</v>
       </c>
-      <c r="P4" s="298" t="s">
+      <c r="P4" s="311" t="s">
         <v>113</v>
       </c>
-      <c r="Q4" s="311" t="s">
+      <c r="Q4" s="307" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="309" t="s">
+      <c r="R4" s="305" t="s">
         <v>114</v>
       </c>
       <c r="S4" s="205" t="s">
@@ -5198,24 +5198,24 @@
       <c r="Y4" s="208"/>
     </row>
     <row r="5" spans="1:26" s="206" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A5" s="306"/>
-      <c r="B5" s="308"/>
-      <c r="C5" s="295"/>
-      <c r="D5" s="295"/>
-      <c r="E5" s="295"/>
-      <c r="F5" s="295"/>
-      <c r="G5" s="295"/>
-      <c r="H5" s="295"/>
-      <c r="I5" s="295"/>
-      <c r="J5" s="295"/>
-      <c r="K5" s="295"/>
-      <c r="L5" s="295"/>
-      <c r="M5" s="295"/>
-      <c r="N5" s="295"/>
-      <c r="O5" s="297"/>
-      <c r="P5" s="299"/>
-      <c r="Q5" s="312"/>
-      <c r="R5" s="310"/>
+      <c r="A5" s="300"/>
+      <c r="B5" s="302"/>
+      <c r="C5" s="304"/>
+      <c r="D5" s="304"/>
+      <c r="E5" s="304"/>
+      <c r="F5" s="304"/>
+      <c r="G5" s="304"/>
+      <c r="H5" s="304"/>
+      <c r="I5" s="304"/>
+      <c r="J5" s="304"/>
+      <c r="K5" s="304"/>
+      <c r="L5" s="304"/>
+      <c r="M5" s="304"/>
+      <c r="N5" s="304"/>
+      <c r="O5" s="310"/>
+      <c r="P5" s="312"/>
+      <c r="Q5" s="308"/>
+      <c r="R5" s="306"/>
       <c r="S5" s="210" t="s">
         <v>115</v>
       </c>
@@ -8606,6 +8606,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -8622,11 +8627,6 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19865,8 +19865,8 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>